<commit_message>
refactor code, rewrote uncommitted code which was lost
</commit_message>
<xml_diff>
--- a/src/data/testData.xlsx
+++ b/src/data/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="232" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="232" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>Username</t>
   </si>
@@ -72,13 +72,13 @@
     <t>Location</t>
   </si>
   <si>
-    <t>M</t>
+    <t>Male</t>
   </si>
   <si>
     <t>person</t>
   </si>
   <si>
-    <t>F</t>
+    <t>Female</t>
   </si>
   <si>
     <t>person1</t>
@@ -99,6 +99,12 @@
     <t>somewhere</t>
   </si>
   <si>
+    <t>person3</t>
+  </si>
+  <si>
+    <t>person3@email.com</t>
+  </si>
+  <si>
     <t>Title</t>
   </si>
   <si>
@@ -135,9 +141,6 @@
     <t>nopassword</t>
   </si>
   <si>
-    <t>yespassword</t>
-  </si>
-  <si>
     <t>whopassword</t>
   </si>
   <si>
@@ -165,9 +168,6 @@
     <t>someemail</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>sds</t>
   </si>
   <si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>email@email.com</t>
-  </si>
-  <si>
-    <t>Male</t>
   </si>
   <si>
     <t>here</t>
@@ -394,10 +391,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -526,10 +523,70 @@
         <v>25</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="person1@email.com"/>
     <hyperlink ref="C4" r:id="rId2" display="person2@gmail.com"/>
+    <hyperlink ref="C5" r:id="rId3" display="person3@email.com"/>
+    <hyperlink ref="C6" r:id="rId4" display="person3@email.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -548,7 +605,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -561,31 +618,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>123</v>
@@ -593,10 +650,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +675,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -631,10 +688,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>14</v>
@@ -645,43 +702,43 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -725,10 +782,10 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
@@ -739,19 +796,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>25</v>
@@ -771,10 +828,10 @@
         <v>51</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,39 +839,39 @@
         <v>342</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3463453</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>